<commit_message>
Implementation of data api on backend and started service on front end.
</commit_message>
<xml_diff>
--- a/sampleDataWithQueries.xlsx
+++ b/sampleDataWithQueries.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sapire-PC\Documents\Design Project 2018\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sapire-PC\Documents\Design Project 2018\DesignProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -913,8 +913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E2:E96"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,8 +963,8 @@
         <v>10</v>
       </c>
       <c r="E2" s="3" t="str">
-        <f t="shared" ref="E2:E33" si="0">"INSERT energyData,sensorName="&amp;$G$2&amp;" kVA="&amp;B2&amp;",kVarh="&amp;C2&amp;",kWh="&amp;D2&amp;" "&amp;((A2-$F$2)*86400000000000)</f>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.46519776082975,kVarh=0.16,kWh=2.46 1514766600000000000</v>
+        <f t="shared" ref="E2:E33" si="0">"INSERT energyData,sensorName="&amp;$G$2&amp;",sensorID=1 kVA="&amp;B2&amp;",kVarh="&amp;C2&amp;",kWh="&amp;D2&amp;" "&amp;((A2-$F$2)*86400000000000)</f>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.46519776082975,kVarh=0.16,kWh=2.46 1514766600000000000</v>
       </c>
       <c r="F2" s="2">
         <v>25569</v>
@@ -988,7 +988,7 @@
       </c>
       <c r="E3" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.46130046926417,kVarh=0.08,kWh=2.46 1514768400000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.46130046926417,kVarh=0.08,kWh=2.46 1514768400000000000</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1006,7 +1006,7 @@
       </c>
       <c r="E4" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.98167738026769,kVarh=0.1,kWh=2.98 1514770200000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.98167738026769,kVarh=0.1,kWh=2.98 1514770200000000000</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1024,7 +1024,7 @@
       </c>
       <c r="E5" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.46519776082975,kVarh=0.16,kWh=2.46 1514772000000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.46519776082975,kVarh=0.16,kWh=2.46 1514772000000000000</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1042,7 +1042,7 @@
       </c>
       <c r="E6" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.36076258865647,kVarh=0.06,kWh=2.36 1514773800000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.36076258865647,kVarh=0.06,kWh=2.36 1514773800000000000</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1060,7 +1060,7 @@
       </c>
       <c r="E7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.53140277316748,kVarh=0.24,kWh=2.52 1514775600000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.53140277316748,kVarh=0.24,kWh=2.52 1514775600000000000</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1078,7 +1078,7 @@
       </c>
       <c r="E8" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.48515593072145,kVarh=0.16,kWh=2.48 1514777400000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.48515593072145,kVarh=0.16,kWh=2.48 1514777400000000000</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1096,7 +1096,7 @@
       </c>
       <c r="E9" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=3.72005376305236,kVarh=0.02,kWh=3.72 1514779200000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=3.72005376305236,kVarh=0.02,kWh=3.72 1514779200000000000</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1114,7 +1114,7 @@
       </c>
       <c r="E10" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=3.30024241533861,kVarh=0.04,kWh=3.3 1514781000000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=3.30024241533861,kVarh=0.04,kWh=3.3 1514781000000000000</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1132,7 +1132,7 @@
       </c>
       <c r="E11" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.48394846967484,kVarh=0.14,kWh=2.48 1514782800000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.48394846967484,kVarh=0.14,kWh=2.48 1514782800000000000</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1150,7 +1150,7 @@
       </c>
       <c r="E12" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=3.26300475022639,kVarh=0.14,kWh=3.26 1514784600000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=3.26300475022639,kVarh=0.14,kWh=3.26 1514784600000000000</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1168,7 +1168,7 @@
       </c>
       <c r="E13" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=1.87882942280559,kVarh=0.38,kWh=1.84 1514786400000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=1.87882942280559,kVarh=0.38,kWh=1.84 1514786400000000000</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1186,7 +1186,7 @@
       </c>
       <c r="E14" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.51435876517254,kVarh=0.52,kWh=2.46 1514788200000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.51435876517254,kVarh=0.52,kWh=2.46 1514788200000000000</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1204,7 +1204,7 @@
       </c>
       <c r="E15" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=1.60162417564171,kVarh=0.44,kWh=1.54 1514790000000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=1.60162417564171,kVarh=0.44,kWh=1.54 1514790000000000000</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1222,7 +1222,7 @@
       </c>
       <c r="E16" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=1.81416647527177,kVarh=0.44,kWh=1.76 1514791800000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=1.81416647527177,kVarh=0.44,kWh=1.76 1514791800000000000</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1240,7 +1240,7 @@
       </c>
       <c r="E17" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=1.57695909902572,kVarh=0.42,kWh=1.52 1514793600000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=1.57695909902572,kVarh=0.42,kWh=1.52 1514793600000000000</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1258,7 +1258,7 @@
       </c>
       <c r="E18" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.18888099265355,kVarh=0.46,kWh=2.14 1514795400000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.18888099265355,kVarh=0.46,kWh=2.14 1514795400000000000</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1276,7 +1276,7 @@
       </c>
       <c r="E19" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=1.73954016912516,kVarh=0.52,kWh=1.66 1514797200000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=1.73954016912516,kVarh=0.52,kWh=1.66 1514797200000000000</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1294,7 +1294,7 @@
       </c>
       <c r="E20" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.43614449489352,kVarh=0.52,kWh=2.38 1514799000000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.43614449489352,kVarh=0.52,kWh=2.38 1514799000000000000</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1312,7 +1312,7 @@
       </c>
       <c r="E21" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.57316925210916,kVarh=0.26,kWh=2.56 1514800800000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.57316925210916,kVarh=0.26,kWh=2.56 1514800800000000000</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1330,7 +1330,7 @@
       </c>
       <c r="E22" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.10646623519106,kVarh=0.44,kWh=2.06 1514802600000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.10646623519106,kVarh=0.44,kWh=2.06 1514802600000000000</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1348,7 +1348,7 @@
       </c>
       <c r="E23" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=1.64012194668567,kVarh=0.44,kWh=1.58 1514804400000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=1.64012194668567,kVarh=0.44,kWh=1.58 1514804400000000000</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1366,7 +1366,7 @@
       </c>
       <c r="E24" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=1.62086396714838,kVarh=0.44,kWh=1.56 1514806200000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=1.62086396714838,kVarh=0.44,kWh=1.56 1514806200000000000</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1384,7 +1384,7 @@
       </c>
       <c r="E25" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=1.61046577113579,kVarh=0.4,kWh=1.56 1514808000000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=1.61046577113579,kVarh=0.4,kWh=1.56 1514808000000000000</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1402,7 +1402,7 @@
       </c>
       <c r="E26" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=1.56204993518133,kVarh=0.36,kWh=1.52 1514809800000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=1.56204993518133,kVarh=0.36,kWh=1.52 1514809800000000000</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1420,7 +1420,7 @@
       </c>
       <c r="E27" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=1.69540555620182,kVarh=0.5,kWh=1.62 1514811600000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=1.69540555620182,kVarh=0.5,kWh=1.62 1514811600000000000</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1438,7 +1438,7 @@
       </c>
       <c r="E28" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=1.61046577113579,kVarh=0.4,kWh=1.56 1514813400000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=1.61046577113579,kVarh=0.4,kWh=1.56 1514813400000000000</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1456,7 +1456,7 @@
       </c>
       <c r="E29" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.46714409793996,kVarh=0.48,kWh=2.42 1514815200000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.46714409793996,kVarh=0.48,kWh=2.42 1514815200000000000</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1474,7 +1474,7 @@
       </c>
       <c r="E30" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.49230816714146,kVarh=0.4,kWh=2.46 1514817000000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.49230816714146,kVarh=0.4,kWh=2.46 1514817000000000000</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1492,7 +1492,7 @@
       </c>
       <c r="E31" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=1.73366663462155,kVarh=0.34,kWh=1.7 1514818800000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=1.73366663462155,kVarh=0.34,kWh=1.7 1514818800000000000</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1510,7 +1510,7 @@
       </c>
       <c r="E32" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=1.87360614858086,kVarh=0.52,kWh=1.8 1514820600000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=1.87360614858086,kVarh=0.52,kWh=1.8 1514820600000000000</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1528,7 +1528,7 @@
       </c>
       <c r="E33" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.37326778935711,kVarh=0.5,kWh=2.32 1514822400000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.37326778935711,kVarh=0.5,kWh=2.32 1514822400000000000</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1545,8 +1545,8 @@
         <v>82</v>
       </c>
       <c r="E34" s="3" t="str">
-        <f t="shared" ref="E34:E65" si="1">"INSERT energyData,sensorName="&amp;$G$2&amp;" kVA="&amp;B34&amp;",kVarh="&amp;C34&amp;",kWh="&amp;D34&amp;" "&amp;((A34-$F$2)*86400000000000)</f>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.65035846632111,kVarh=0.4,kWh=2.62 1514824200000000000</v>
+        <f t="shared" ref="E34:E65" si="1">"INSERT energyData,sensorName="&amp;$G$2&amp;",sensorID=1 kVA="&amp;B34&amp;",kVarh="&amp;C34&amp;",kWh="&amp;D34&amp;" "&amp;((A34-$F$2)*86400000000000)</f>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.65035846632111,kVarh=0.4,kWh=2.62 1514824200000000000</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1564,7 +1564,7 @@
       </c>
       <c r="E35" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=1.73954016912516,kVarh=0.52,kWh=1.66 1514826000000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=1.73954016912516,kVarh=0.52,kWh=1.66 1514826000000000000</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1582,7 +1582,7 @@
       </c>
       <c r="E36" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=1.95058965443786,kVarh=0.52,kWh=1.88 1514827800000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=1.95058965443786,kVarh=0.52,kWh=1.88 1514827800000000000</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1600,7 +1600,7 @@
       </c>
       <c r="E37" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=1.97686620690425,kVarh=0.38,kWh=1.94 1514829600000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=1.97686620690425,kVarh=0.38,kWh=1.94 1514829600000000000</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1618,7 +1618,7 @@
       </c>
       <c r="E38" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.33117995873334,kVarh=0.38,kWh=2.3 1514831400000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.33117995873334,kVarh=0.38,kWh=2.3 1514831400000000000</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1636,7 +1636,7 @@
       </c>
       <c r="E39" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=3.91003836298316,kVarh=0.28,kWh=3.9 1514833200000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=3.91003836298316,kVarh=0.28,kWh=3.9 1514833200000000000</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1654,7 +1654,7 @@
       </c>
       <c r="E40" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=3.0841530441922,kVarh=0.16,kWh=3.08 1514835000000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=3.0841530441922,kVarh=0.16,kWh=3.08 1514835000000000000</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1672,7 +1672,7 @@
       </c>
       <c r="E41" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.76354844357757,kVarh=0.14,kWh=2.76 1514836800000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.76354844357757,kVarh=0.14,kWh=2.76 1514836800000000000</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1690,7 +1690,7 @@
       </c>
       <c r="E42" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=3.28219438790575,kVarh=0.12,kWh=3.28 1514838600000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=3.28219438790575,kVarh=0.12,kWh=3.28 1514838600000000000</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1708,7 +1708,7 @@
       </c>
       <c r="E43" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=3.28152403617587,kVarh=0.1,kWh=3.28 1514840400000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=3.28152403617587,kVarh=0.1,kWh=3.28 1514840400000000000</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1726,7 +1726,7 @@
       </c>
       <c r="E44" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=3.98246155034798,kVarh=0.14,kWh=3.98 1514842200000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=3.98246155034798,kVarh=0.14,kWh=3.98 1514842200000000000</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1744,7 +1744,7 @@
       </c>
       <c r="E45" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=4.02019900004962,kVarh=0.04,kWh=4.02 1514844000000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=4.02019900004962,kVarh=0.04,kWh=4.02 1514844000000000000</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1762,7 +1762,7 @@
       </c>
       <c r="E46" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.80349781523011,kVarh=0.14,kWh=2.8 1514845800000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.80349781523011,kVarh=0.14,kWh=2.8 1514845800000000000</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1780,7 +1780,7 @@
       </c>
       <c r="E47" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=4.08078423835419,kVarh=0.08,kWh=4.08 1514847600000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=4.08078423835419,kVarh=0.08,kWh=4.08 1514847600000000000</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1798,7 +1798,7 @@
       </c>
       <c r="E48" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=4.06177301187548,kVarh=0.12,kWh=4.06 1514849400000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=4.06177301187548,kVarh=0.12,kWh=4.06 1514849400000000000</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1816,7 +1816,7 @@
       </c>
       <c r="E49" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.50071989634985,kVarh=0.06,kWh=2.5 1514851200000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.50071989634985,kVarh=0.06,kWh=2.5 1514851200000000000</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1834,7 +1834,7 @@
       </c>
       <c r="E50" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.62373779177722,kVarh=0.14,kWh=2.62 1514853000000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.62373779177722,kVarh=0.14,kWh=2.62 1514853000000000000</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1852,7 +1852,7 @@
       </c>
       <c r="E51" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=3.06104557300279,kVarh=0.08,kWh=3.06 1514854800000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=3.06104557300279,kVarh=0.08,kWh=3.06 1514854800000000000</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1870,7 +1870,7 @@
       </c>
       <c r="E52" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.62373779177722,kVarh=0.14,kWh=2.62 1514856600000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.62373779177722,kVarh=0.14,kWh=2.62 1514856600000000000</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1888,7 +1888,7 @@
       </c>
       <c r="E53" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.70599334810712,kVarh=0.18,kWh=2.7 1514858400000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.70599334810712,kVarh=0.18,kWh=2.7 1514858400000000000</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1906,7 +1906,7 @@
       </c>
       <c r="E54" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=3.08058436014987,kVarh=0.06,kWh=3.08 1514860200000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=3.08058436014987,kVarh=0.06,kWh=3.08 1514860200000000000</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -1924,7 +1924,7 @@
       </c>
       <c r="E55" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=4.84004132213765,kVarh=0.02,kWh=4.84 1514862000000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=4.84004132213765,kVarh=0.02,kWh=4.84 1514862000000000000</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -1942,7 +1942,7 @@
       </c>
       <c r="E56" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=3.32054212441282,kVarh=0.06,kWh=3.32 1514863800000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=3.32054212441282,kVarh=0.06,kWh=3.32 1514863800000000000</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="E57" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=3.44093010681705,kVarh=0.08,kWh=3.44 1514865600000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=3.44093010681705,kVarh=0.08,kWh=3.44 1514865600000000000</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -1978,7 +1978,7 @@
       </c>
       <c r="E58" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=4.26168980569914,kVarh=0.12,kWh=4.26 1514867400000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=4.26168980569914,kVarh=0.12,kWh=4.26 1514867400000000000</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -1996,7 +1996,7 @@
       </c>
       <c r="E59" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=3.30024241533861,kVarh=0.04,kWh=3.3 1514869200000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=3.30024241533861,kVarh=0.04,kWh=3.3 1514869200000000000</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -2014,7 +2014,7 @@
       </c>
       <c r="E60" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=3.88046388979462,kVarh=0.06,kWh=3.88 1514871000000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=3.88046388979462,kVarh=0.06,kWh=3.88 1514871000000000000</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -2032,7 +2032,7 @@
       </c>
       <c r="E61" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.65035846632111,kVarh=0.4,kWh=2.62 1514872800000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.65035846632111,kVarh=0.4,kWh=2.62 1514872800000000000</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -2050,7 +2050,7 @@
       </c>
       <c r="E62" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.922259399848,kVarh=0.36,kWh=2.9 1514874600000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.922259399848,kVarh=0.36,kWh=2.9 1514874600000000000</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -2068,7 +2068,7 @@
       </c>
       <c r="E63" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.05922315449298,kVarh=0.4,kWh=2.02 1514876400000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.05922315449298,kVarh=0.4,kWh=2.02 1514876400000000000</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -2086,7 +2086,7 @@
       </c>
       <c r="E64" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=1.7464249196573,kVarh=0.4,kWh=1.7 1514878200000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=1.7464249196573,kVarh=0.4,kWh=1.7 1514878200000000000</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -2104,7 +2104,7 @@
       </c>
       <c r="E65" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=1.67487312952355,kVarh=0.34,kWh=1.64 1514880000000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=1.67487312952355,kVarh=0.34,kWh=1.64 1514880000000000000</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -2121,8 +2121,8 @@
         <v>137</v>
       </c>
       <c r="E66" s="3" t="str">
-        <f t="shared" ref="E66:E97" si="2">"INSERT energyData,sensorName="&amp;$G$2&amp;" kVA="&amp;B66&amp;",kVarh="&amp;C66&amp;",kWh="&amp;D66&amp;" "&amp;((A66-$F$2)*86400000000000)</f>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.90496127340796,kVarh=0.38,kWh=2.88 1514881800000000000</v>
+        <f t="shared" ref="E66:E97" si="2">"INSERT energyData,sensorName="&amp;$G$2&amp;",sensorID=1 kVA="&amp;B66&amp;",kVarh="&amp;C66&amp;",kWh="&amp;D66&amp;" "&amp;((A66-$F$2)*86400000000000)</f>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.90496127340796,kVarh=0.38,kWh=2.88 1514881800000000000</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -2140,7 +2140,7 @@
       </c>
       <c r="E67" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.08278659492517,kVarh=0.42,kWh=2.04 1514883600000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.08278659492517,kVarh=0.42,kWh=2.04 1514883600000000000</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -2158,7 +2158,7 @@
       </c>
       <c r="E68" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.01613491612045,kVarh=0.38,kWh=1.98 1514885400000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.01613491612045,kVarh=0.38,kWh=1.98 1514885400000000000</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -2176,7 +2176,7 @@
       </c>
       <c r="E69" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=3.99809954853553,kVarh=0.38,kWh=3.98 1514887200000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=3.99809954853553,kVarh=0.38,kWh=3.98 1514887200000000000</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -2194,7 +2194,7 @@
       </c>
       <c r="E70" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.58495647932417,kVarh=0.48,kWh=2.54 1514889000000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.58495647932417,kVarh=0.48,kWh=2.54 1514889000000000000</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -2212,7 +2212,7 @@
       </c>
       <c r="E71" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=3.33736422944814,kVarh=0.34,kWh=3.32 1514890800000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=3.33736422944814,kVarh=0.34,kWh=3.32 1514890800000000000</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -2230,7 +2230,7 @@
       </c>
       <c r="E72" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=4.13937193303525,kVarh=0.4,kWh=4.12 1514892600000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=4.13937193303525,kVarh=0.4,kWh=4.12 1514892600000000000</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -2248,7 +2248,7 @@
       </c>
       <c r="E73" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.26274169979695,kVarh=0.32,kWh=2.24 1514894400000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.26274169979695,kVarh=0.32,kWh=2.24 1514894400000000000</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -2266,7 +2266,7 @@
       </c>
       <c r="E74" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=1.88743211798464,kVarh=0.5,kWh=1.82 1514896200000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=1.88743211798464,kVarh=0.5,kWh=1.82 1514896200000000000</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -2284,7 +2284,7 @@
       </c>
       <c r="E75" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.02237484161567,kVarh=0.3,kWh=2 1514898000000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.02237484161567,kVarh=0.3,kWh=2 1514898000000000000</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -2302,7 +2302,7 @@
       </c>
       <c r="E76" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=1.77538728169377,kVarh=0.44,kWh=1.72 1514899800000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=1.77538728169377,kVarh=0.44,kWh=1.72 1514899800000000000</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -2320,7 +2320,7 @@
       </c>
       <c r="E77" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=1.67355908171776,kVarh=0.42,kWh=1.62 1514901600000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=1.67355908171776,kVarh=0.42,kWh=1.62 1514901600000000000</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -2338,7 +2338,7 @@
       </c>
       <c r="E78" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=1.86783296897769,kVarh=0.42,kWh=1.82 1514903400000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=1.86783296897769,kVarh=0.42,kWh=1.82 1514903400000000000</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -2356,7 +2356,7 @@
       </c>
       <c r="E79" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.36719242986285,kVarh=0.56,kWh=2.3 1514905200000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.36719242986285,kVarh=0.56,kWh=2.3 1514905200000000000</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -2374,7 +2374,7 @@
       </c>
       <c r="E80" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=1.67487312952355,kVarh=0.34,kWh=1.64 1514907000000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=1.67487312952355,kVarh=0.34,kWh=1.64 1514907000000000000</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -2392,7 +2392,7 @@
       </c>
       <c r="E81" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.01791972090071,kVarh=0.48,kWh=1.96 1514908800000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.01791972090071,kVarh=0.48,kWh=1.96 1514908800000000000</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -2410,7 +2410,7 @@
       </c>
       <c r="E82" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.9698484809835,kVarh=0.42,kWh=2.94 1514910600000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.9698484809835,kVarh=0.42,kWh=2.94 1514910600000000000</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -2428,7 +2428,7 @@
       </c>
       <c r="E83" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=1.72244012958361,kVarh=0.38,kWh=1.68 1514912400000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=1.72244012958361,kVarh=0.38,kWh=1.68 1514912400000000000</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -2446,7 +2446,7 @@
       </c>
       <c r="E84" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.1377558326432,kVarh=0.4,kWh=2.1 1514914200000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.1377558326432,kVarh=0.4,kWh=2.1 1514914200000000000</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -2464,7 +2464,7 @@
       </c>
       <c r="E85" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.41238471227124,kVarh=0.5,kWh=2.36 1514916000000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.41238471227124,kVarh=0.5,kWh=2.36 1514916000000000000</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -2482,7 +2482,7 @@
       </c>
       <c r="E86" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.59976922052708,kVarh=0.32,kWh=2.58 1514917800000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.59976922052708,kVarh=0.32,kWh=2.58 1514917800000000000</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -2500,7 +2500,7 @@
       </c>
       <c r="E87" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.20045449850707,kVarh=0.42,kWh=2.16 1514919600000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.20045449850707,kVarh=0.42,kWh=2.16 1514919600000000000</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -2518,7 +2518,7 @@
       </c>
       <c r="E88" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=4.68346025925277,kVarh=0.18,kWh=4.68 1514921400000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=4.68346025925277,kVarh=0.18,kWh=4.68 1514921400000000000</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -2536,7 +2536,7 @@
       </c>
       <c r="E89" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.60622332120638,kVarh=0.18,kWh=2.6 1514923200000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.60622332120638,kVarh=0.18,kWh=2.6 1514923200000000000</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -2554,7 +2554,7 @@
       </c>
       <c r="E90" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.94333144582801,kVarh=0.14,kWh=2.94 1514925000000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.94333144582801,kVarh=0.14,kWh=2.94 1514925000000000000</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -2572,7 +2572,7 @@
       </c>
       <c r="E91" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.34136712200372,kVarh=0.08,kWh=2.34 1514926800000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.34136712200372,kVarh=0.08,kWh=2.34 1514926800000000000</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -2590,7 +2590,7 @@
       </c>
       <c r="E92" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=3.08103878586427,kVarh=0.08,kWh=3.08 1514928600000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=3.08103878586427,kVarh=0.08,kWh=3.08 1514928600000000000</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -2608,7 +2608,7 @@
       </c>
       <c r="E93" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.7435743110038,kVarh=0.14,kWh=2.74 1514930400000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.7435743110038,kVarh=0.14,kWh=2.74 1514930400000000000</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -2626,7 +2626,7 @@
       </c>
       <c r="E94" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=2.70473658606527,kVarh=0.16,kWh=2.7 1514932200000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.70473658606527,kVarh=0.16,kWh=2.7 1514932200000000000</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -2644,7 +2644,7 @@
       </c>
       <c r="E95" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=3.88082465463205,kVarh=0.08,kWh=3.88 1514934000000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=3.88082465463205,kVarh=0.08,kWh=3.88 1514934000000000000</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -2662,10 +2662,11 @@
       </c>
       <c r="E96" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>INSERT energyData,sensorName=WITS13JubileeRoad kVA=3.72134384329102,kVarh=0.1,kWh=3.72 1514935800000000000</v>
+        <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=3.72134384329102,kVarh=0.1,kWh=3.72 1514935800000000000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding canvas.js graphing framework. Implemented data representation user story. Added basic sensor and data infrastructures.
</commit_message>
<xml_diff>
--- a/sampleDataWithQueries.xlsx
+++ b/sampleDataWithQueries.xlsx
@@ -913,15 +913,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E96"/>
+    <sheetView tabSelected="1" topLeftCell="E85" workbookViewId="0">
+      <selection activeCell="E96" sqref="E96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" customWidth="1"/>
     <col min="2" max="2" width="18.5703125" customWidth="1"/>
-    <col min="5" max="5" width="105.5703125" customWidth="1"/>
+    <col min="5" max="5" width="123.5703125" customWidth="1"/>
     <col min="6" max="6" width="15.42578125" customWidth="1"/>
     <col min="7" max="7" width="18.7109375" customWidth="1"/>
   </cols>
@@ -2121,7 +2121,7 @@
         <v>137</v>
       </c>
       <c r="E66" s="3" t="str">
-        <f t="shared" ref="E66:E97" si="2">"INSERT energyData,sensorName="&amp;$G$2&amp;",sensorID=1 kVA="&amp;B66&amp;",kVarh="&amp;C66&amp;",kWh="&amp;D66&amp;" "&amp;((A66-$F$2)*86400000000000)</f>
+        <f t="shared" ref="E66:E96" si="2">"INSERT energyData,sensorName="&amp;$G$2&amp;",sensorID=1 kVA="&amp;B66&amp;",kVarh="&amp;C66&amp;",kWh="&amp;D66&amp;" "&amp;((A66-$F$2)*86400000000000)</f>
         <v>INSERT energyData,sensorName=WITS13JubileeRoad,sensorID=1 kVA=2.90496127340796,kVarh=0.38,kWh=2.88 1514881800000000000</v>
       </c>
     </row>

</xml_diff>